<commit_message>
[MOSIP-42349] Added script to update the google spreadsheet through csv
Signed-off-by: ckm007 <chandrakeshavmishra@gmail.com>
</commit_message>
<xml_diff>
--- a/minio-report-tracker/xlxs/cellbox21.xlsx
+++ b/minio-report-tracker/xlxs/cellbox21.xlsx
@@ -406,31 +406,6 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>242</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="7620000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="12" name="Image 12" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -723,7 +698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,8 +709,8 @@
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="6" customWidth="1" min="4" max="4"/>
-    <col width="5" customWidth="1" min="5" max="5"/>
+    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="6" customWidth="1" min="5" max="5"/>
     <col width="5" customWidth="1" min="6" max="6"/>
     <col width="4" customWidth="1" min="7" max="7"/>
     <col width="4" customWidth="1" min="8" max="8"/>
@@ -785,27 +760,27 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45849</v>
+        <v>45867</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>auth</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>512</v>
+        <v>410</v>
       </c>
       <c r="D2" t="n">
-        <v>198</v>
+        <v>320</v>
       </c>
       <c r="E2" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>153</v>
+        <v>6</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -813,27 +788,27 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45848</v>
+        <v>45866</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>auth</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>512</v>
+        <v>410</v>
       </c>
       <c r="D3" t="n">
-        <v>492</v>
+        <v>320</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -841,27 +816,27 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45847</v>
+        <v>45865</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>auth</t>
+          <t>dsl</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>512</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>491</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -869,27 +844,27 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45846</v>
+        <v>45864</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>auth</t>
+          <t>dsl</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>512</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>492</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -897,27 +872,27 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45845</v>
+        <v>45863</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>auth</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>512</v>
+        <v>410</v>
       </c>
       <c r="D6" t="n">
-        <v>493</v>
+        <v>320</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -925,27 +900,27 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45849</v>
+        <v>45867</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>idrepo</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>410</v>
+        <v>945</v>
       </c>
       <c r="D7" t="n">
-        <v>322</v>
+        <v>920</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -953,27 +928,27 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45848</v>
+        <v>45866</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>idrepo</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>410</v>
+        <v>945</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>920</v>
       </c>
       <c r="E8" t="n">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -981,27 +956,27 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45847</v>
+        <v>45863</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>idrepo</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>410</v>
+        <v>945</v>
       </c>
       <c r="D9" t="n">
-        <v>322</v>
+        <v>920</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1009,27 +984,27 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45846</v>
+        <v>45867</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>idrepo</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>410</v>
+        <v>945</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>935</v>
       </c>
       <c r="E10" t="n">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1037,27 +1012,27 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45845</v>
+        <v>45866</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>idrepo</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>410</v>
+        <v>945</v>
       </c>
       <c r="D11" t="n">
-        <v>322</v>
+        <v>935</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1065,18 +1040,18 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45849</v>
+        <v>45863</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>945</v>
       </c>
       <c r="D12" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1085,7 +1060,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1093,11 +1068,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45848</v>
+        <v>45867</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -1121,11 +1096,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45847</v>
+        <v>45866</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1149,11 +1124,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45846</v>
+        <v>45863</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1177,11 +1152,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>45845</v>
+        <v>45867</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1205,18 +1180,18 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>45849</v>
+        <v>45866</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>945</v>
       </c>
       <c r="D17" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1225,7 +1200,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1233,18 +1208,18 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45848</v>
+        <v>45863</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>945</v>
       </c>
       <c r="D18" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1253,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1261,18 +1236,18 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45847</v>
+        <v>45867</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>945</v>
       </c>
       <c r="D19" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -1281,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -1289,18 +1264,18 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45846</v>
+        <v>45866</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>945</v>
       </c>
       <c r="D20" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1309,7 +1284,7 @@
         <v>10</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
@@ -1317,18 +1292,18 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>45845</v>
+        <v>45863</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>945</v>
       </c>
       <c r="D21" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1337,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1345,11 +1320,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>45849</v>
+        <v>45867</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1373,11 +1348,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45848</v>
+        <v>45866</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1401,11 +1376,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45847</v>
+        <v>45863</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1429,111 +1404,111 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45846</v>
+        <v>45867</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>945</v>
+        <v>509</v>
       </c>
       <c r="D25" t="n">
-        <v>920</v>
+        <v>332</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F25" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G25" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>45845</v>
+        <v>45866</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>945</v>
+        <v>509</v>
       </c>
       <c r="D26" t="n">
-        <v>920</v>
+        <v>332</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F26" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G26" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>45849</v>
+        <v>45863</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>945</v>
+        <v>509</v>
       </c>
       <c r="D27" t="n">
-        <v>920</v>
+        <v>332</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F27" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G27" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>45848</v>
+        <v>45867</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>prereg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>945</v>
+        <v>281</v>
       </c>
       <c r="D28" t="n">
-        <v>920</v>
+        <v>206</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="G28" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1541,27 +1516,27 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>45847</v>
+        <v>45866</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>prereg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>945</v>
+        <v>281</v>
       </c>
       <c r="D29" t="n">
-        <v>920</v>
+        <v>54</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="F29" t="n">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="G29" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
         <v>0</v>
@@ -1569,27 +1544,27 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>45846</v>
+        <v>45863</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>prereg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>945</v>
+        <v>281</v>
       </c>
       <c r="D30" t="n">
-        <v>920</v>
+        <v>224</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F30" t="n">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="G30" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>0</v>
@@ -1597,27 +1572,27 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45845</v>
+        <v>45867</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>resident</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>945</v>
+        <v>1126</v>
       </c>
       <c r="D31" t="n">
-        <v>920</v>
+        <v>895</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F31" t="n">
-        <v>10</v>
+        <v>183</v>
       </c>
       <c r="G31" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1625,27 +1600,27 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45849</v>
+        <v>45866</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>resident</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>945</v>
+        <v>1126</v>
       </c>
       <c r="D32" t="n">
-        <v>920</v>
+        <v>842</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F32" t="n">
-        <v>10</v>
+        <v>272</v>
       </c>
       <c r="G32" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1653,27 +1628,27 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>45848</v>
+        <v>45863</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>resident</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>945</v>
+        <v>1126</v>
       </c>
       <c r="D33" t="n">
-        <v>920</v>
+        <v>31</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>1046</v>
       </c>
       <c r="F33" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="G33" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1681,27 +1656,27 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45847</v>
+        <v>45867</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>dsl</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>945</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>920</v>
+        <v>3</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1709,27 +1684,27 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>45846</v>
+        <v>45866</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>dsl</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>945</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>920</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
         <v>0</v>
@@ -1737,673 +1712,29 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>45845</v>
+        <v>45863</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>dsl</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>945</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>920</v>
+        <v>2</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>945</v>
-      </c>
-      <c r="D37" t="n">
-        <v>920</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>10</v>
-      </c>
-      <c r="G37" t="n">
-        <v>15</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>45848</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>945</v>
-      </c>
-      <c r="D38" t="n">
-        <v>920</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>10</v>
-      </c>
-      <c r="G38" t="n">
-        <v>15</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="C39" t="n">
-        <v>945</v>
-      </c>
-      <c r="D39" t="n">
-        <v>920</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>10</v>
-      </c>
-      <c r="G39" t="n">
-        <v>15</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>45846</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>945</v>
-      </c>
-      <c r="D40" t="n">
-        <v>920</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>10</v>
-      </c>
-      <c r="G40" t="n">
-        <v>15</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="C41" t="n">
-        <v>945</v>
-      </c>
-      <c r="D41" t="n">
-        <v>920</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>10</v>
-      </c>
-      <c r="G41" t="n">
-        <v>15</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>509</v>
-      </c>
-      <c r="D42" t="n">
-        <v>332</v>
-      </c>
-      <c r="E42" t="n">
-        <v>134</v>
-      </c>
-      <c r="F42" t="n">
-        <v>31</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0</v>
-      </c>
-      <c r="H42" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>45848</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>509</v>
-      </c>
-      <c r="D43" t="n">
-        <v>332</v>
-      </c>
-      <c r="E43" t="n">
-        <v>134</v>
-      </c>
-      <c r="F43" t="n">
-        <v>31</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
-      <c r="H43" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>509</v>
-      </c>
-      <c r="D44" t="n">
-        <v>332</v>
-      </c>
-      <c r="E44" t="n">
-        <v>134</v>
-      </c>
-      <c r="F44" t="n">
-        <v>31</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>45846</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>509</v>
-      </c>
-      <c r="D45" t="n">
-        <v>332</v>
-      </c>
-      <c r="E45" t="n">
-        <v>134</v>
-      </c>
-      <c r="F45" t="n">
-        <v>31</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>509</v>
-      </c>
-      <c r="D46" t="n">
-        <v>497</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0</v>
-      </c>
-      <c r="H46" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="C47" t="n">
-        <v>288</v>
-      </c>
-      <c r="D47" t="n">
-        <v>280</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>6</v>
-      </c>
-      <c r="G47" t="n">
-        <v>2</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>45848</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>288</v>
-      </c>
-      <c r="D48" t="n">
-        <v>280</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>6</v>
-      </c>
-      <c r="G48" t="n">
-        <v>2</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>288</v>
-      </c>
-      <c r="D49" t="n">
-        <v>280</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>6</v>
-      </c>
-      <c r="G49" t="n">
-        <v>2</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>45846</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>288</v>
-      </c>
-      <c r="D50" t="n">
-        <v>280</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>6</v>
-      </c>
-      <c r="G50" t="n">
-        <v>2</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>288</v>
-      </c>
-      <c r="D51" t="n">
-        <v>280</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>6</v>
-      </c>
-      <c r="G51" t="n">
-        <v>2</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>45849</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>dsl</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>197</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="n">
-        <v>195</v>
-      </c>
-      <c r="F52" t="n">
-        <v>2</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>45848</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>resident</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D53" t="n">
-        <v>874</v>
-      </c>
-      <c r="E53" t="n">
-        <v>12</v>
-      </c>
-      <c r="F53" t="n">
-        <v>240</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>resident</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D54" t="n">
-        <v>880</v>
-      </c>
-      <c r="E54" t="n">
-        <v>12</v>
-      </c>
-      <c r="F54" t="n">
-        <v>234</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>45846</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>resident</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1106</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>20</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>resident</t>
-        </is>
-      </c>
-      <c r="C56" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1117</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
-        <v>9</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>45847</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>dsl</t>
-        </is>
-      </c>
-      <c r="C57" t="n">
-        <v>3</v>
-      </c>
-      <c r="D57" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" t="n">
-        <v>1</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>45846</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>dsl</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>3</v>
-      </c>
-      <c r="D58" t="n">
-        <v>3</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>45845</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>dsl</t>
-        </is>
-      </c>
-      <c r="C59" t="n">
-        <v>3</v>
-      </c>
-      <c r="D59" t="n">
-        <v>2</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
-        <v>1</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CSV, XLSX, and Google Sheet reports
</commit_message>
<xml_diff>
--- a/minio-report-tracker/xlxs/cellbox21.xlsx
+++ b/minio-report-tracker/xlxs/cellbox21.xlsx
@@ -712,14 +712,14 @@
     <col width="5" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="5" customWidth="1" min="6" max="6"/>
-    <col width="4" customWidth="1" min="7" max="7"/>
-    <col width="4" customWidth="1" min="8" max="8"/>
+    <col width="5" customWidth="1" min="7" max="7"/>
+    <col width="5" customWidth="1" min="8" max="8"/>
     <col width="2" customWidth="1" min="9" max="9"/>
     <col width="14" customWidth="1" min="10" max="10"/>
     <col width="16" customWidth="1" min="11" max="11"/>
     <col width="6" customWidth="1" min="12" max="12"/>
     <col width="5" customWidth="1" min="13" max="13"/>
-    <col width="5" customWidth="1" min="14" max="14"/>
+    <col width="6" customWidth="1" min="14" max="14"/>
     <col width="5" customWidth="1" min="15" max="15"/>
     <col width="4" customWidth="1" min="16" max="16"/>
     <col width="4" customWidth="1" min="17" max="17"/>
@@ -737,8 +737,8 @@
     <col width="16" customWidth="1" min="29" max="29"/>
     <col width="6" customWidth="1" min="30" max="30"/>
     <col width="5" customWidth="1" min="31" max="31"/>
-    <col width="6" customWidth="1" min="32" max="32"/>
-    <col width="4" customWidth="1" min="33" max="33"/>
+    <col width="5" customWidth="1" min="32" max="32"/>
+    <col width="5" customWidth="1" min="33" max="33"/>
     <col width="4" customWidth="1" min="34" max="34"/>
     <col width="4" customWidth="1" min="35" max="35"/>
     <col width="2" customWidth="1" min="36" max="36"/>
@@ -747,7 +747,7 @@
     <col width="6" customWidth="1" min="39" max="39"/>
     <col width="5" customWidth="1" min="40" max="40"/>
     <col width="6" customWidth="1" min="41" max="41"/>
-    <col width="5" customWidth="1" min="42" max="42"/>
+    <col width="4" customWidth="1" min="42" max="42"/>
     <col width="4" customWidth="1" min="43" max="43"/>
     <col width="4" customWidth="1" min="44" max="44"/>
   </cols>
@@ -957,197 +957,197 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>idrepo</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>410</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>idrepo</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>410</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>326</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>84</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>idrepo</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>410</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>320</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>84</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>idrepo</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>410</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>320</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>84</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>25-July-2025</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>idrepo</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>410</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>320</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>84</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
-        </is>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>idrepo</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>410</t>
-        </is>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
-          <t>410</t>
-        </is>
-      </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="AR2" t="inlineStr">
@@ -1159,167 +1159,167 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>masterdata-ara</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>920</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>masterdata-ara</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>masterdata-ara</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="AC3" t="inlineStr">
         <is>
           <t>masterdata-ara</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="AD3" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="AE3" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="AH3" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>masterdata-ara</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>920</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
@@ -1361,167 +1361,167 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>masterdata-eng</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>935</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>masterdata-eng</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>935</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>masterdata-eng</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>935</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="AC4" t="inlineStr">
         <is>
           <t>masterdata-eng</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="AD4" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="AE4" t="inlineStr">
         <is>
           <t>935</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>masterdata-eng</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>935</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
@@ -1563,192 +1563,192 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>masterdata-fra</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>920</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>masterdata-fra</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>masterdata-fra</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Y5" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="AC5" t="inlineStr">
         <is>
           <t>masterdata-fra</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="AD5" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="AE5" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="AH5" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
         <is>
           <t>25-July-2025</t>
         </is>
       </c>
-      <c r="AC5" t="inlineStr">
+      <c r="AL5" t="inlineStr">
         <is>
           <t>masterdata-fra</t>
         </is>
       </c>
-      <c r="AD5" t="inlineStr">
+      <c r="AM5" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AN5" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
         <is>
           <t>10</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>masterdata-fra</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr">
-        <is>
-          <t>919</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>11</t>
         </is>
       </c>
       <c r="AQ5" t="inlineStr">
@@ -1765,167 +1765,167 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>masterdata-hin</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>920</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>masterdata-hin</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>masterdata-hin</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Y6" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="AC6" t="inlineStr">
         <is>
           <t>masterdata-hin</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="AD6" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V6" t="inlineStr">
+      <c r="AE6" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="AH6" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>masterdata-hin</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>920</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
@@ -1967,167 +1967,167 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>masterdata-kan</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>920</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>masterdata-kan</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>masterdata-kan</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Y7" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="AC7" t="inlineStr">
         <is>
           <t>masterdata-kan</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
+      <c r="AD7" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V7" t="inlineStr">
+      <c r="AE7" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
+      <c r="AH7" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>masterdata-kan</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>920</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
@@ -2169,167 +2169,167 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>masterdata-tam</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>919</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>masterdata-tam</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>masterdata-tam</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Y8" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="AC8" t="inlineStr">
         <is>
           <t>masterdata-tam</t>
         </is>
       </c>
-      <c r="U8" t="inlineStr">
+      <c r="AD8" t="inlineStr">
         <is>
           <t>945</t>
         </is>
       </c>
-      <c r="V8" t="inlineStr">
+      <c r="AE8" t="inlineStr">
         <is>
           <t>920</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
+      <c r="AH8" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>masterdata-tam</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>920</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
@@ -2371,167 +2371,167 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>509</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>332</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>134</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>pms</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>509</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>332</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>134</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="T9" t="inlineStr">
         <is>
           <t>pms</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="U9" t="inlineStr">
         <is>
           <t>509</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="V9" t="inlineStr">
         <is>
           <t>332</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="W9" t="inlineStr">
         <is>
           <t>134</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="X9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="AB9" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="AC9" t="inlineStr">
         <is>
           <t>pms</t>
         </is>
       </c>
-      <c r="U9" t="inlineStr">
+      <c r="AD9" t="inlineStr">
         <is>
           <t>509</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr">
+      <c r="AE9" t="inlineStr">
         <is>
           <t>332</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
+      <c r="AF9" t="inlineStr">
         <is>
           <t>134</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr">
+      <c r="AG9" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr">
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="AB9" t="inlineStr">
+      <c r="AK9" t="inlineStr">
         <is>
           <t>25-July-2025</t>
-        </is>
-      </c>
-      <c r="AC9" t="inlineStr">
-        <is>
-          <t>pms</t>
-        </is>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t>509</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>332</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>134</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="AH9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI9" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="AK9" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
         </is>
       </c>
       <c r="AL9" t="inlineStr">
@@ -2573,192 +2573,192 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1126</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>1126</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>prereg</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>281</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>206</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>71</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="T10" t="inlineStr">
         <is>
           <t>prereg</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="U10" t="inlineStr">
         <is>
           <t>281</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="V10" t="inlineStr">
         <is>
           <t>206</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="W10" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="X10" t="inlineStr">
         <is>
           <t>71</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="AC10" t="inlineStr">
         <is>
           <t>prereg</t>
         </is>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="AD10" t="inlineStr">
         <is>
           <t>281</t>
         </is>
       </c>
-      <c r="V10" t="inlineStr">
+      <c r="AE10" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="AF10" t="inlineStr">
         <is>
           <t>129</t>
         </is>
       </c>
-      <c r="X10" t="inlineStr">
+      <c r="AG10" t="inlineStr">
         <is>
           <t>98</t>
         </is>
       </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
+      <c r="AH10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
         <is>
           <t>25-July-2025</t>
         </is>
       </c>
-      <c r="AC10" t="inlineStr">
+      <c r="AL10" t="inlineStr">
         <is>
           <t>prereg</t>
         </is>
       </c>
-      <c r="AD10" t="inlineStr">
+      <c r="AM10" t="inlineStr">
         <is>
           <t>281</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr">
+      <c r="AN10" t="inlineStr">
         <is>
           <t>224</t>
         </is>
       </c>
-      <c r="AF10" t="inlineStr">
+      <c r="AO10" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="AG10" t="inlineStr">
+      <c r="AP10" t="inlineStr">
         <is>
           <t>53</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK10" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
-        </is>
-      </c>
-      <c r="AL10" t="inlineStr">
-        <is>
-          <t>prereg</t>
-        </is>
-      </c>
-      <c r="AM10" t="inlineStr">
-        <is>
-          <t>281</t>
-        </is>
-      </c>
-      <c r="AN10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AO10" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
-      </c>
-      <c r="AP10" t="inlineStr">
-        <is>
-          <t>206</t>
         </is>
       </c>
       <c r="AQ10" t="inlineStr">
@@ -2775,192 +2775,192 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>31-July-2025</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>resident</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>1126</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>1033</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>62</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>resident</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>1126</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="V11" t="inlineStr">
         <is>
           <t>895</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="W11" t="inlineStr">
         <is>
           <t>48</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="X11" t="inlineStr">
         <is>
           <t>183</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="AC11" t="inlineStr">
         <is>
           <t>resident</t>
         </is>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="AD11" t="inlineStr">
         <is>
           <t>1126</t>
         </is>
       </c>
-      <c r="V11" t="inlineStr">
+      <c r="AE11" t="inlineStr">
         <is>
           <t>842</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="AF11" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="X11" t="inlineStr">
+      <c r="AG11" t="inlineStr">
         <is>
           <t>272</t>
         </is>
       </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
         <is>
           <t>25-July-2025</t>
         </is>
       </c>
-      <c r="AC11" t="inlineStr">
+      <c r="AL11" t="inlineStr">
         <is>
           <t>resident</t>
         </is>
       </c>
-      <c r="AD11" t="inlineStr">
+      <c r="AM11" t="inlineStr">
         <is>
           <t>1126</t>
         </is>
       </c>
-      <c r="AE11" t="inlineStr">
+      <c r="AN11" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="AF11" t="inlineStr">
+      <c r="AO11" t="inlineStr">
         <is>
           <t>1046</t>
         </is>
       </c>
-      <c r="AG11" t="inlineStr">
+      <c r="AP11" t="inlineStr">
         <is>
           <t>49</t>
-        </is>
-      </c>
-      <c r="AH11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
-        </is>
-      </c>
-      <c r="AL11" t="inlineStr">
-        <is>
-          <t>resident</t>
-        </is>
-      </c>
-      <c r="AM11" t="inlineStr">
-        <is>
-          <t>1126</t>
-        </is>
-      </c>
-      <c r="AN11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AO11" t="inlineStr">
-        <is>
-          <t>1126</t>
-        </is>
-      </c>
-      <c r="AP11" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
       <c r="AQ11" t="inlineStr">
@@ -2975,194 +2975,178 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v/>
+      </c>
+      <c r="B12" t="n">
+        <v/>
+      </c>
+      <c r="C12" t="n">
+        <v/>
+      </c>
+      <c r="D12" t="n">
+        <v/>
+      </c>
+      <c r="E12" t="n">
+        <v/>
+      </c>
+      <c r="F12" t="n">
+        <v/>
+      </c>
+      <c r="G12" t="n">
+        <v/>
+      </c>
+      <c r="H12" t="n">
+        <v/>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>30-July-2025</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>197</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>34</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>163</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>29-July-2025</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="T12" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="U12" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="V12" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
         <is>
           <t>28-July-2025</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="AC12" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="AD12" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="W12" t="inlineStr">
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="X12" t="inlineStr">
+      <c r="AG12" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AB12" t="inlineStr">
+      <c r="AH12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
         <is>
           <t>25-July-2025</t>
         </is>
       </c>
-      <c r="AC12" t="inlineStr">
+      <c r="AL12" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="AD12" t="inlineStr">
+      <c r="AM12" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="AE12" t="inlineStr">
+      <c r="AN12" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AF12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG12" t="inlineStr">
+      <c r="AO12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP12" t="inlineStr">
         <is>
           <t>1</t>
-        </is>
-      </c>
-      <c r="AH12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AI12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AK12" t="inlineStr">
-        <is>
-          <t>23-July-2025</t>
-        </is>
-      </c>
-      <c r="AL12" t="inlineStr">
-        <is>
-          <t>dsl</t>
-        </is>
-      </c>
-      <c r="AM12" t="inlineStr">
-        <is>
-          <t>197</t>
-        </is>
-      </c>
-      <c r="AN12" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AO12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AP12" t="inlineStr">
-        <is>
-          <t>191</t>
         </is>
       </c>
       <c r="AQ12" t="inlineStr">

</xml_diff>